<commit_message>
Toegevoegd Activity Diagram Control Washing Cycle
</commit_message>
<xml_diff>
--- a/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
+++ b/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>Omschrijving activiteit</t>
   </si>
@@ -254,13 +254,28 @@
     <t>Donderdag Vergadering</t>
   </si>
   <si>
-    <t>Maandag 11:30 tot 15:00 werkbijeenkomst</t>
-  </si>
-  <si>
     <t>Deadline Requirement voor 23:59</t>
   </si>
   <si>
     <t>Deadline inleveren plan van aanpak voor 23:59</t>
+  </si>
+  <si>
+    <t>Maandag Maken Constraints</t>
+  </si>
+  <si>
+    <t>Maandag Maken Activity Diagram Control washing cycle</t>
+  </si>
+  <si>
+    <t>Maandag Maken Activity Diagram Provide access</t>
+  </si>
+  <si>
+    <t>Maandag Maken Activity Diagram Manage user profile</t>
+  </si>
+  <si>
+    <t>Maandag Maken Activity Diagram Display machine state</t>
+  </si>
+  <si>
+    <t>Maandag Maken Activity Diagram Read machine state</t>
   </si>
 </sst>
 </file>
@@ -422,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -531,6 +546,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -856,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -899,24 +917,24 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51" t="s">
+      <c r="D3" s="51"/>
+      <c r="E3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="52" t="s">
+      <c r="F3" s="52"/>
+      <c r="G3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="51" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="51"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="49"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="50"/>
       <c r="M3" s="26" t="s">
         <v>9</v>
       </c>
@@ -1611,189 +1629,259 @@
         <v>4</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C22" s="21">
-        <v>3.5</v>
-      </c>
-      <c r="D22" s="21"/>
+        <v>2</v>
+      </c>
+      <c r="D22" s="21">
+        <v>2</v>
+      </c>
       <c r="E22" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="F22" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
       <c r="G22" s="16">
-        <v>3.5</v>
-      </c>
-      <c r="H22" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="16">
+        <v>0</v>
+      </c>
       <c r="I22" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="J22" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="30">
-        <f t="shared" si="5"/>
-        <v>14</v>
+        <f>C22+E22+G22+I22+K22</f>
+        <v>2</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" ref="N21:N22" si="6">D22+F22+H22+J22+L22</f>
-        <v>0</v>
+        <f t="shared" ref="N22:N26" si="6">D22+F22+H22+J22+L22</f>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="25">
+      <c r="A23" s="48">
         <v>4</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C23" s="21">
-        <v>2</v>
-      </c>
-      <c r="D23" s="21"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="21">
+        <v>0</v>
+      </c>
       <c r="E23" s="2">
-        <v>2</v>
-      </c>
-      <c r="F23" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
       <c r="G23" s="16">
-        <v>2</v>
-      </c>
-      <c r="H23" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0</v>
+      </c>
       <c r="I23" s="2">
-        <v>2</v>
-      </c>
-      <c r="J23" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="30">
-        <f t="shared" ref="M23:N53" si="7">C23+E23+G23+I23+K23</f>
-        <v>8</v>
+        <f>C23+E23+G23+I23+K23</f>
+        <v>1</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="A24" s="48">
         <v>4</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C24" s="21">
-        <v>3</v>
-      </c>
-      <c r="D24" s="21"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="21">
+        <v>0</v>
+      </c>
       <c r="E24" s="2">
-        <v>3</v>
-      </c>
-      <c r="F24" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
       <c r="G24" s="16">
-        <v>3</v>
-      </c>
-      <c r="H24" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="16">
+        <v>0</v>
+      </c>
       <c r="I24" s="2">
-        <v>3</v>
-      </c>
-      <c r="J24" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="30">
-        <f t="shared" ref="M24:M26" si="8">C24+E24+G24+I24+K24</f>
-        <v>12</v>
+        <f>C24+E24+G24+I24+K24</f>
+        <v>1</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" ref="N24:N26" si="9">D24+F24+H24+J24+L24</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="25">
+      <c r="A25" s="48">
         <v>4</v>
       </c>
-      <c r="B25" s="44" t="s">
-        <v>34</v>
+      <c r="B25" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="C25" s="21">
-        <v>1</v>
-      </c>
-      <c r="D25" s="21"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="21">
+        <v>0</v>
+      </c>
       <c r="E25" s="2">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
       <c r="G25" s="16">
-        <v>1</v>
-      </c>
-      <c r="H25" s="16"/>
+        <v>2</v>
+      </c>
+      <c r="H25" s="16">
+        <v>2</v>
+      </c>
       <c r="I25" s="2">
-        <v>1</v>
-      </c>
-      <c r="J25" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="30">
         <f>C25+E25+G25+I25+K25</f>
+        <v>2</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="48">
         <v>4</v>
       </c>
-      <c r="N25" s="2">
-        <f>D25+F25+H25+J25+L25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="25">
-        <v>4</v>
-      </c>
-      <c r="B26" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="B26" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="21">
+        <v>0</v>
+      </c>
+      <c r="D26" s="21">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="16">
+        <v>0</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>2</v>
+      </c>
+      <c r="J26" s="2">
+        <v>2</v>
+      </c>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="30">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f>C26+E26+G26+I26+K26</f>
+        <v>2</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="47">
+      <c r="A27" s="25">
         <v>4</v>
       </c>
-      <c r="B27" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
+      <c r="B27" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="D27" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G27" s="16">
+        <v>1.5</v>
+      </c>
+      <c r="H27" s="16">
+        <v>1.5</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1.5</v>
+      </c>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="2"/>
+      <c r="M27" s="30">
+        <f t="shared" ref="M27:N57" si="7">C27+E27+G27+I27+K27</f>
+        <v>6</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C28" s="21">
         <v>2</v>
@@ -1808,59 +1896,61 @@
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="30">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" ref="M28:M30" si="8">C28+E28+G28+I28+K28</f>
+        <v>8</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="N28:N30" si="9">D28+F28+H28+J28+L28</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="25">
-        <v>5</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>34</v>
       </c>
       <c r="C29" s="21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H29" s="16"/>
       <c r="I29" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="30">
-        <f t="shared" ref="M29:N30" si="10">C29+E29+G29+I29+K29</f>
-        <v>12</v>
+        <f>C29+E29+G29+I29+K29</f>
+        <v>4</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="10"/>
+        <f>D29+F29+H29+J29+L29</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="25">
-        <v>5</v>
-      </c>
-      <c r="B30" s="12"/>
+        <v>4</v>
+      </c>
+      <c r="B30" s="45" t="s">
+        <v>40</v>
+      </c>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
       <c r="E30" s="2"/>
@@ -1872,76 +1962,62 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="M30" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N30" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>6</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="21">
-        <v>2</v>
-      </c>
+      <c r="A31" s="47">
+        <v>4</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="21"/>
       <c r="D31" s="21"/>
-      <c r="E31" s="2">
-        <v>2</v>
-      </c>
+      <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="16">
-        <v>2</v>
-      </c>
+      <c r="G31" s="16"/>
       <c r="H31" s="16"/>
-      <c r="I31" s="2">
-        <v>0</v>
-      </c>
+      <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
-      <c r="M31" s="30">
-        <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="N31" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="M31" s="30"/>
+      <c r="N31" s="2"/>
     </row>
     <row r="32" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>6</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="22">
-        <v>3</v>
-      </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="1">
-        <v>3</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="17">
-        <v>3</v>
-      </c>
-      <c r="H32" s="17"/>
-      <c r="I32" s="1">
-        <v>3</v>
-      </c>
-      <c r="J32" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="21">
+        <v>2</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="16">
+        <v>2</v>
+      </c>
+      <c r="H32" s="16"/>
+      <c r="I32" s="2">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="M32" s="30">
         <f t="shared" si="7"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N32" s="2">
         <f t="shared" si="7"/>
@@ -1949,50 +2025,60 @@
       </c>
     </row>
     <row r="33" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>6</v>
-      </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="A33" s="25">
+        <v>5</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="21">
+        <v>3</v>
+      </c>
+      <c r="D33" s="21"/>
+      <c r="E33" s="2">
+        <v>3</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="16">
+        <v>3</v>
+      </c>
+      <c r="H33" s="16"/>
+      <c r="I33" s="2">
+        <v>3</v>
+      </c>
+      <c r="J33" s="2"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
       <c r="M33" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" ref="M33:N34" si="10">C33+E33+G33+I33+K33</f>
+        <v>12</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>6</v>
+      <c r="A34" s="25">
+        <v>5</v>
       </c>
       <c r="B34" s="12"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="M34" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N34" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -2000,22 +2086,30 @@
       <c r="A35" s="1">
         <v>6</v>
       </c>
-      <c r="B35" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="B35" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="21">
+        <v>2</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="2">
+        <v>2</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="16">
+        <v>2</v>
+      </c>
+      <c r="H35" s="16"/>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="30">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N35" s="2">
         <f t="shared" si="7"/>
@@ -2023,80 +2117,116 @@
       </c>
     </row>
     <row r="36" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
+      <c r="A36" s="1">
+        <v>6</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="22">
+        <v>3</v>
+      </c>
+      <c r="D36" s="22"/>
+      <c r="E36" s="1">
+        <v>3</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="17">
+        <v>3</v>
+      </c>
+      <c r="H36" s="17"/>
+      <c r="I36" s="1">
+        <v>3</v>
+      </c>
+      <c r="J36" s="1"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="2"/>
+      <c r="M36" s="30">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="40" t="s">
-        <v>22</v>
+      <c r="A37" s="1">
+        <v>6</v>
       </c>
       <c r="B37" s="12"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="2"/>
+      <c r="M37" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="40" t="s">
-        <v>22</v>
+      <c r="A38" s="1">
+        <v>6</v>
       </c>
       <c r="B38" s="12"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="2"/>
+      <c r="M38" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="40"/>
-      <c r="J39" s="40"/>
+      <c r="A39" s="1">
+        <v>6</v>
+      </c>
+      <c r="B39" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="2"/>
+      <c r="M39" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="39"/>
@@ -2114,7 +2244,7 @@
     </row>
     <row r="41" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="39"/>
@@ -2131,103 +2261,79 @@
       <c r="N41" s="2"/>
     </row>
     <row r="42" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>12</v>
+      <c r="A42" s="40" t="s">
+        <v>22</v>
       </c>
       <c r="B42" s="12"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
-      <c r="M42" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N42" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="M42" s="30"/>
+      <c r="N42" s="2"/>
     </row>
     <row r="43" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="28" t="s">
-        <v>12</v>
+      <c r="A43" s="40" t="s">
+        <v>23</v>
       </c>
       <c r="B43" s="12"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
-      <c r="M43" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N43" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="M43" s="30"/>
+      <c r="N43" s="2"/>
     </row>
     <row r="44" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="28" t="s">
-        <v>12</v>
+      <c r="A44" s="40" t="s">
+        <v>23</v>
       </c>
       <c r="B44" s="12"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
-      <c r="M44" s="30">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N44" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="28" t="s">
-        <v>12</v>
+      <c r="M44" s="30"/>
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="40" t="s">
+        <v>23</v>
       </c>
       <c r="B45" s="12"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
-      <c r="M45" s="30">
-        <f t="shared" ref="M45:M54" si="11">C45+E45+G45+I45+K45</f>
-        <v>0</v>
-      </c>
-      <c r="N45" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="28" t="s">
+      <c r="M45" s="30"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B46" s="12"/>
@@ -2242,7 +2348,7 @@
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N46" s="2">
@@ -2250,7 +2356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="28" t="s">
         <v>12</v>
       </c>
@@ -2266,7 +2372,7 @@
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
       <c r="M47" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N47" s="2">
@@ -2274,9 +2380,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>13</v>
+    <row r="48" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="28" t="s">
+        <v>12</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="22"/>
@@ -2290,7 +2396,7 @@
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
       <c r="M48" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N48" s="2">
@@ -2300,7 +2406,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="22"/>
@@ -2314,7 +2420,7 @@
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
       <c r="M49" s="30">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="M49:M58" si="11">C49+E49+G49+I49+K49</f>
         <v>0</v>
       </c>
       <c r="N49" s="2">
@@ -2324,9 +2430,9 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="13"/>
+        <v>12</v>
+      </c>
+      <c r="B50" s="12"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
       <c r="E50" s="1"/>
@@ -2348,7 +2454,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="22"/>
@@ -2371,7 +2477,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B52" s="12"/>
@@ -2398,9 +2504,7 @@
       <c r="A53" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="45" t="s">
-        <v>29</v>
-      </c>
+      <c r="B53" s="12"/>
       <c r="C53" s="22"/>
       <c r="D53" s="22"/>
       <c r="E53" s="1"/>
@@ -2421,75 +2525,173 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A54" s="10"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
+      <c r="A54" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
-      <c r="M54" s="31">
+      <c r="M54" s="30">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N54" s="11"/>
+      <c r="N54" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A55" s="32"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="34">
-        <f>SUM(C5:C54)</f>
-        <v>40.5</v>
-      </c>
-      <c r="D55" s="34">
-        <f>SUM(D5:D54)</f>
-        <v>20</v>
-      </c>
-      <c r="E55" s="34">
-        <f>SUM(E5:E54)</f>
-        <v>40.5</v>
-      </c>
-      <c r="F55" s="34">
-        <f>SUM(F5:F54)</f>
-        <v>18</v>
-      </c>
-      <c r="G55" s="34">
-        <f>SUM(G5:G54)</f>
-        <v>40.5</v>
-      </c>
-      <c r="H55" s="34">
-        <f>SUM(H5:H54)</f>
-        <v>20</v>
-      </c>
-      <c r="I55" s="34">
-        <f>SUM(I5:I54)</f>
-        <v>32.5</v>
-      </c>
-      <c r="J55" s="34">
-        <f>SUM(J5:J54)</f>
-        <v>16</v>
-      </c>
-      <c r="K55" s="34"/>
-      <c r="L55" s="34"/>
-      <c r="M55" s="32">
-        <f>C55+E55+G55+I55+K55</f>
-        <v>154</v>
-      </c>
-      <c r="N55" s="34">
-        <f>D55+F55+H55+J55+L55</f>
-        <v>74</v>
+      <c r="A55" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="12"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="30">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N55" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B56" s="33" t="s">
+      <c r="A56" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="12"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="30">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N56" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="30">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N57" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" s="10"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="31">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N58" s="11"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" s="32"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="34">
+        <f t="shared" ref="C59:J59" si="12">SUM(C5:C58)</f>
+        <v>37.5</v>
+      </c>
+      <c r="D59" s="34">
+        <f t="shared" si="12"/>
+        <v>23.5</v>
+      </c>
+      <c r="E59" s="34">
+        <f t="shared" si="12"/>
+        <v>37.5</v>
+      </c>
+      <c r="F59" s="34">
+        <f t="shared" si="12"/>
+        <v>21.5</v>
+      </c>
+      <c r="G59" s="34">
+        <f t="shared" si="12"/>
+        <v>37.5</v>
+      </c>
+      <c r="H59" s="34">
+        <f t="shared" si="12"/>
+        <v>23.5</v>
+      </c>
+      <c r="I59" s="34">
+        <f t="shared" si="12"/>
+        <v>29.5</v>
+      </c>
+      <c r="J59" s="34">
+        <f t="shared" si="12"/>
+        <v>19.5</v>
+      </c>
+      <c r="K59" s="34"/>
+      <c r="L59" s="34"/>
+      <c r="M59" s="32">
+        <f>C59+E59+G59+I59+K59</f>
+        <v>142</v>
+      </c>
+      <c r="N59" s="34">
+        <f>D59+F59+H59+J59+L59</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B60" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="K56" s="43"/>
+      <c r="K60" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2523,25 +2725,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
-    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
-    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D777D35650D3B43A23D41664AA30BC5" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="7f80e5700d93aba1c148b391c267eb5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ab5e87a-ed8e-45a5-9793-059f67398425" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e36a552b910c1cdf142adc90bba5ebe9" ns2:_="">
     <xsd:import namespace="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
@@ -2702,35 +2885,30 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
+    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
+    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6B4BC2B-47EC-4A4E-997D-A663CFE6E409}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2748,6 +2926,30 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
uren en agenda toegevoegd
</commit_message>
<xml_diff>
--- a/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
+++ b/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
@@ -365,9 +365,6 @@
     <t>Donderdag vergadering 15:00</t>
   </si>
   <si>
-    <t>Donderdag maken STD's</t>
-  </si>
-  <si>
     <t>Vrijdag PvA</t>
   </si>
   <si>
@@ -378,6 +375,9 @@
   </si>
   <si>
     <t>Dinsdag Maken klassendiagram</t>
+  </si>
+  <si>
+    <t>Donderdag bijwerken RA en SA</t>
   </si>
 </sst>
 </file>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1277,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="20">
         <v>0</v>
@@ -1589,7 +1589,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="20">
         <v>0</v>
@@ -2651,13 +2651,13 @@
         <v>0.5</v>
       </c>
       <c r="H43" s="16">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="I43" s="2">
         <v>0.5</v>
       </c>
       <c r="J43" s="2">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
@@ -2667,25 +2667,46 @@
       </c>
       <c r="N43" s="2">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="64"/>
+      <c r="A44" s="64">
+        <v>5</v>
+      </c>
       <c r="B44" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="C44" s="21">
+        <v>0</v>
+      </c>
+      <c r="D44" s="21">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0</v>
+      </c>
+      <c r="G44" s="16">
+        <v>0</v>
+      </c>
+      <c r="H44" s="16">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2">
+        <v>1</v>
+      </c>
+      <c r="J44" s="2">
+        <v>1</v>
+      </c>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
-      <c r="M44" s="30"/>
+      <c r="M44" s="30">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
       <c r="N44" s="2"/>
     </row>
     <row r="45" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2787,7 +2808,7 @@
         <v>6</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C48" s="63">
         <v>0</v>
@@ -2810,7 +2831,9 @@
       <c r="I48" s="64">
         <v>1.5</v>
       </c>
-      <c r="J48" s="64"/>
+      <c r="J48" s="64">
+        <v>1.5</v>
+      </c>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
       <c r="M48" s="30"/>
@@ -2826,19 +2849,27 @@
       <c r="C49" s="49">
         <v>0.5</v>
       </c>
-      <c r="D49" s="49"/>
+      <c r="D49" s="49">
+        <v>0.5</v>
+      </c>
       <c r="E49" s="50">
         <v>0.5</v>
       </c>
-      <c r="F49" s="50"/>
+      <c r="F49" s="50">
+        <v>0.5</v>
+      </c>
       <c r="G49" s="51">
         <v>0</v>
       </c>
-      <c r="H49" s="51"/>
+      <c r="H49" s="51">
+        <v>0</v>
+      </c>
       <c r="I49" s="50">
         <v>0.5</v>
       </c>
-      <c r="J49" s="50"/>
+      <c r="J49" s="50">
+        <v>0.5</v>
+      </c>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
       <c r="M49" s="30"/>
@@ -2849,24 +2880,32 @@
         <v>6</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C50" s="22">
         <v>0.5</v>
       </c>
-      <c r="D50" s="22"/>
+      <c r="D50" s="22">
+        <v>1.5</v>
+      </c>
       <c r="E50" s="1">
         <v>0.5</v>
       </c>
-      <c r="F50" s="1"/>
+      <c r="F50" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G50" s="17">
         <v>0</v>
       </c>
-      <c r="H50" s="17"/>
+      <c r="H50" s="17">
+        <v>0</v>
+      </c>
       <c r="I50" s="1">
         <v>0.5</v>
       </c>
-      <c r="J50" s="1"/>
+      <c r="J50" s="1">
+        <v>1.5</v>
+      </c>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
       <c r="M50" s="30">
@@ -2875,7 +2914,7 @@
       </c>
       <c r="N50" s="2">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="51" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2888,19 +2927,27 @@
       <c r="C51" s="60">
         <v>2</v>
       </c>
-      <c r="D51" s="60"/>
+      <c r="D51" s="60">
+        <v>1</v>
+      </c>
       <c r="E51" s="61">
         <v>2</v>
       </c>
-      <c r="F51" s="61"/>
+      <c r="F51" s="61">
+        <v>1</v>
+      </c>
       <c r="G51" s="62">
         <v>0</v>
       </c>
-      <c r="H51" s="62"/>
+      <c r="H51" s="62">
+        <v>0</v>
+      </c>
       <c r="I51" s="61">
         <v>2</v>
       </c>
-      <c r="J51" s="61"/>
+      <c r="J51" s="61">
+        <v>1</v>
+      </c>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
       <c r="M51" s="30"/>
@@ -3008,19 +3055,19 @@
         <v>48</v>
       </c>
       <c r="C55" s="39">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D55" s="39"/>
       <c r="E55" s="40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F55" s="40"/>
       <c r="G55" s="41">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H55" s="41"/>
       <c r="I55" s="40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J55" s="40"/>
       <c r="K55" s="8"/>
@@ -3728,45 +3775,45 @@
       <c r="B80" s="10"/>
       <c r="C80" s="34">
         <f t="shared" ref="C80:J80" si="12">SUM(C5:C79)</f>
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D80" s="34">
         <f t="shared" si="12"/>
-        <v>40.5</v>
+        <v>43.5</v>
       </c>
       <c r="E80" s="34">
         <f t="shared" si="12"/>
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F80" s="34">
         <f t="shared" si="12"/>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G80" s="34">
         <f t="shared" si="12"/>
-        <v>123.5</v>
+        <v>125.5</v>
       </c>
       <c r="H80" s="34">
         <f t="shared" si="12"/>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I80" s="34">
         <f t="shared" si="12"/>
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J80" s="34">
         <f t="shared" si="12"/>
-        <v>33.5</v>
+        <v>41</v>
       </c>
       <c r="K80" s="34"/>
       <c r="L80" s="34"/>
       <c r="M80" s="32">
         <f>C80+E80+G80+I80+K80</f>
-        <v>516.5</v>
+        <v>520.5</v>
       </c>
       <c r="N80" s="34">
         <f>D80+F80+H80+J80+L80</f>
-        <v>150</v>
+        <v>165.5</v>
       </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Agenda en Urenverandwoording bijgewerkt
</commit_message>
<xml_diff>
--- a/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
+++ b/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="84">
   <si>
     <t>Omschrijving activiteit</t>
   </si>
@@ -378,6 +378,15 @@
   </si>
   <si>
     <t>Donderdag bijwerken RA en SA</t>
+  </si>
+  <si>
+    <t>Tentamen</t>
+  </si>
+  <si>
+    <t>Dinsdag verbeteren SA diagrammen</t>
+  </si>
+  <si>
+    <t>Donderdag Hardware optimaliseren</t>
   </si>
 </sst>
 </file>
@@ -551,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -698,6 +707,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1037,15 +1055,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N81"/>
+  <dimension ref="A1:N83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="54.140625" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
@@ -1080,24 +1098,24 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69" t="s">
+      <c r="D3" s="71"/>
+      <c r="E3" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="69"/>
-      <c r="G3" s="70" t="s">
+      <c r="F3" s="72"/>
+      <c r="G3" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="I3" s="69" t="s">
+      <c r="H3" s="73"/>
+      <c r="I3" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="69"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="67"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="70"/>
       <c r="M3" s="26" t="s">
         <v>9</v>
       </c>
@@ -2109,7 +2127,7 @@
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="30">
-        <f t="shared" ref="M29:N78" si="7">C29+E29+G29+I29+K29</f>
+        <f t="shared" ref="M29:N80" si="7">C29+E29+G29+I29+K29</f>
         <v>6</v>
       </c>
       <c r="N29" s="2">
@@ -3029,19 +3047,27 @@
       <c r="C54" s="39">
         <v>0</v>
       </c>
-      <c r="D54" s="39"/>
+      <c r="D54" s="39">
+        <v>0</v>
+      </c>
       <c r="E54" s="40">
         <v>0</v>
       </c>
-      <c r="F54" s="40"/>
+      <c r="F54" s="40">
+        <v>0</v>
+      </c>
       <c r="G54" s="41">
         <v>0</v>
       </c>
-      <c r="H54" s="41"/>
+      <c r="H54" s="41">
+        <v>0</v>
+      </c>
       <c r="I54" s="40">
         <v>3</v>
       </c>
-      <c r="J54" s="40"/>
+      <c r="J54" s="40">
+        <v>2</v>
+      </c>
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
       <c r="M54" s="30"/>
@@ -3057,19 +3083,27 @@
       <c r="C55" s="39">
         <v>5</v>
       </c>
-      <c r="D55" s="39"/>
+      <c r="D55" s="39">
+        <v>0</v>
+      </c>
       <c r="E55" s="40">
         <v>5</v>
       </c>
-      <c r="F55" s="40"/>
+      <c r="F55" s="40">
+        <v>0</v>
+      </c>
       <c r="G55" s="41">
         <v>5</v>
       </c>
-      <c r="H55" s="41"/>
+      <c r="H55" s="41">
+        <v>0</v>
+      </c>
       <c r="I55" s="40">
         <v>0</v>
       </c>
-      <c r="J55" s="40"/>
+      <c r="J55" s="40">
+        <v>0</v>
+      </c>
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
       <c r="M55" s="30"/>
@@ -3085,19 +3119,27 @@
       <c r="C56" s="39">
         <v>4</v>
       </c>
-      <c r="D56" s="39"/>
+      <c r="D56" s="39">
+        <v>0</v>
+      </c>
       <c r="E56" s="40">
         <v>4</v>
       </c>
-      <c r="F56" s="40"/>
+      <c r="F56" s="40">
+        <v>0</v>
+      </c>
       <c r="G56" s="41">
         <v>4</v>
       </c>
-      <c r="H56" s="41"/>
+      <c r="H56" s="41">
+        <v>0</v>
+      </c>
       <c r="I56" s="40">
         <v>4</v>
       </c>
-      <c r="J56" s="40"/>
+      <c r="J56" s="40">
+        <v>0</v>
+      </c>
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
       <c r="M56" s="30"/>
@@ -3107,7 +3149,9 @@
       <c r="A57" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B57" s="12"/>
+      <c r="B57" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="C57" s="39"/>
       <c r="D57" s="39"/>
       <c r="E57" s="40"/>
@@ -3125,7 +3169,9 @@
       <c r="A58" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B58" s="12"/>
+      <c r="B58" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="C58" s="39"/>
       <c r="D58" s="39"/>
       <c r="E58" s="40"/>
@@ -3143,7 +3189,9 @@
       <c r="A59" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B59" s="12"/>
+      <c r="B59" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="C59" s="39"/>
       <c r="D59" s="39"/>
       <c r="E59" s="40"/>
@@ -3158,200 +3206,210 @@
       <c r="N59" s="2"/>
     </row>
     <row r="60" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="50"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="49"/>
-      <c r="D60" s="49"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="50"/>
-      <c r="G60" s="51"/>
-      <c r="H60" s="51"/>
-      <c r="I60" s="50"/>
-      <c r="J60" s="50"/>
+      <c r="A60" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C60" s="66">
+        <v>2</v>
+      </c>
+      <c r="D60" s="66">
+        <v>2</v>
+      </c>
+      <c r="E60" s="67">
+        <v>0</v>
+      </c>
+      <c r="F60" s="67">
+        <v>0</v>
+      </c>
+      <c r="G60" s="68">
+        <v>0</v>
+      </c>
+      <c r="H60" s="68">
+        <v>0</v>
+      </c>
+      <c r="I60" s="67">
+        <v>1.5</v>
+      </c>
+      <c r="J60" s="67">
+        <v>1.5</v>
+      </c>
       <c r="K60" s="8"/>
       <c r="L60" s="8"/>
       <c r="M60" s="30"/>
       <c r="N60" s="2"/>
     </row>
     <row r="61" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>12</v>
+      <c r="A61" s="67" t="s">
+        <v>81</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C61" s="22">
-        <v>1</v>
-      </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="1">
-        <v>0</v>
-      </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="17">
-        <v>0</v>
-      </c>
-      <c r="H61" s="17"/>
-      <c r="I61" s="1">
-        <v>0</v>
-      </c>
-      <c r="J61" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="C61" s="66">
+        <v>0</v>
+      </c>
+      <c r="D61" s="66">
+        <v>0</v>
+      </c>
+      <c r="E61" s="67">
+        <v>0</v>
+      </c>
+      <c r="F61" s="67">
+        <v>0</v>
+      </c>
+      <c r="G61" s="68">
+        <v>0</v>
+      </c>
+      <c r="H61" s="68">
+        <v>0</v>
+      </c>
+      <c r="I61" s="67">
+        <v>1</v>
+      </c>
+      <c r="J61" s="67">
+        <v>1</v>
+      </c>
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
-      <c r="M61" s="30">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="N61" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="M61" s="30"/>
+      <c r="N61" s="2"/>
     </row>
     <row r="62" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C62" s="22">
-        <v>7</v>
-      </c>
-      <c r="D62" s="22"/>
-      <c r="E62" s="1">
-        <v>8</v>
-      </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="17">
-        <v>8</v>
-      </c>
-      <c r="H62" s="17"/>
-      <c r="I62" s="1">
-        <v>8</v>
-      </c>
-      <c r="J62" s="1"/>
+      <c r="A62" s="50"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="50"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="50"/>
+      <c r="J62" s="50"/>
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
-      <c r="M62" s="30">
+      <c r="M62" s="30"/>
+      <c r="N62" s="2"/>
+    </row>
+    <row r="63" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" s="22">
+        <v>1</v>
+      </c>
+      <c r="D63" s="22"/>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1"/>
+      <c r="G63" s="17">
+        <v>0</v>
+      </c>
+      <c r="H63" s="17"/>
+      <c r="I63" s="1">
+        <v>0</v>
+      </c>
+      <c r="J63" s="1"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="30">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N63" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C64" s="22">
+        <v>7</v>
+      </c>
+      <c r="D64" s="22"/>
+      <c r="E64" s="1">
+        <v>8</v>
+      </c>
+      <c r="F64" s="1"/>
+      <c r="G64" s="17">
+        <v>8</v>
+      </c>
+      <c r="H64" s="17"/>
+      <c r="I64" s="1">
+        <v>8</v>
+      </c>
+      <c r="J64" s="1"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="8"/>
+      <c r="M64" s="30">
         <f t="shared" si="7"/>
         <v>31</v>
       </c>
-      <c r="N62" s="2">
+      <c r="N64" s="2">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="50" t="s">
+    <row r="65" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B65" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="49">
-        <v>2</v>
-      </c>
-      <c r="D63" s="49"/>
-      <c r="E63" s="50">
-        <v>2</v>
-      </c>
-      <c r="F63" s="50"/>
-      <c r="G63" s="51">
-        <v>2</v>
-      </c>
-      <c r="H63" s="51"/>
-      <c r="I63" s="50">
-        <v>2</v>
-      </c>
-      <c r="J63" s="50"/>
-      <c r="K63" s="8"/>
-      <c r="L63" s="8"/>
-      <c r="M63" s="30"/>
-      <c r="N63" s="2"/>
-    </row>
-    <row r="64" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C64" s="49">
-        <v>6</v>
-      </c>
-      <c r="D64" s="49"/>
-      <c r="E64" s="50">
-        <v>6</v>
-      </c>
-      <c r="F64" s="50"/>
-      <c r="G64" s="51">
-        <v>6</v>
-      </c>
-      <c r="H64" s="51"/>
-      <c r="I64" s="50">
-        <v>6</v>
-      </c>
-      <c r="J64" s="50"/>
-      <c r="K64" s="8"/>
-      <c r="L64" s="8"/>
-      <c r="M64" s="30"/>
-      <c r="N64" s="2"/>
-    </row>
-    <row r="65" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C65" s="22">
-        <v>0</v>
-      </c>
-      <c r="D65" s="22"/>
-      <c r="E65" s="1">
-        <v>1</v>
-      </c>
-      <c r="F65" s="1"/>
-      <c r="G65" s="17">
-        <v>0</v>
-      </c>
-      <c r="H65" s="17"/>
-      <c r="I65" s="1">
-        <v>0</v>
-      </c>
-      <c r="J65" s="1"/>
+      <c r="C65" s="49">
+        <v>2</v>
+      </c>
+      <c r="D65" s="49"/>
+      <c r="E65" s="50">
+        <v>2</v>
+      </c>
+      <c r="F65" s="50"/>
+      <c r="G65" s="51">
+        <v>2</v>
+      </c>
+      <c r="H65" s="51"/>
+      <c r="I65" s="50">
+        <v>2</v>
+      </c>
+      <c r="J65" s="50"/>
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
-      <c r="M65" s="30">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="N65" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="M65" s="30"/>
+      <c r="N65" s="2"/>
     </row>
     <row r="66" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="50" t="s">
         <v>12</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C66" s="49">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D66" s="49"/>
       <c r="E66" s="50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" s="50"/>
       <c r="G66" s="51">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H66" s="51"/>
       <c r="I66" s="50">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J66" s="50"/>
       <c r="K66" s="8"/>
@@ -3359,23 +3417,23 @@
       <c r="M66" s="30"/>
       <c r="N66" s="2"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C67" s="22">
         <v>0</v>
       </c>
       <c r="D67" s="22"/>
       <c r="E67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" s="17"/>
       <c r="I67" s="1">
@@ -3385,7 +3443,7 @@
       <c r="K67" s="8"/>
       <c r="L67" s="8"/>
       <c r="M67" s="30">
-        <f t="shared" ref="M67:M79" si="11">C67+E67+G67+I67+K67</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N67" s="2">
@@ -3393,23 +3451,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="50" t="s">
         <v>12</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C68" s="49">
         <v>8</v>
       </c>
       <c r="D68" s="49"/>
       <c r="E68" s="50">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" s="50"/>
       <c r="G68" s="51">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H68" s="51"/>
       <c r="I68" s="50">
@@ -3418,10 +3476,7 @@
       <c r="J68" s="50"/>
       <c r="K68" s="8"/>
       <c r="L68" s="8"/>
-      <c r="M68" s="30">
-        <f t="shared" si="11"/>
-        <v>31</v>
-      </c>
+      <c r="M68" s="30"/>
       <c r="N68" s="2"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -3429,29 +3484,29 @@
         <v>12</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C69" s="22">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D69" s="22"/>
       <c r="E69" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="17">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H69" s="17"/>
       <c r="I69" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J69" s="1"/>
       <c r="K69" s="8"/>
       <c r="L69" s="8"/>
       <c r="M69" s="30">
-        <f t="shared" si="11"/>
-        <v>32</v>
+        <f t="shared" ref="M69:M81" si="11">C69+E69+G69+I69+K69</f>
+        <v>1</v>
       </c>
       <c r="N69" s="2">
         <f t="shared" si="7"/>
@@ -3459,83 +3514,98 @@
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A70" s="28" t="s">
+      <c r="A70" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="B70" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C70" s="54">
-        <v>0</v>
-      </c>
-      <c r="D70" s="22"/>
-      <c r="E70" s="1">
-        <v>0</v>
-      </c>
-      <c r="F70" s="1"/>
-      <c r="G70" s="17">
-        <v>0</v>
-      </c>
-      <c r="H70" s="17"/>
-      <c r="I70" s="1">
-        <v>0</v>
-      </c>
-      <c r="J70" s="1"/>
+      <c r="B70" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C70" s="49">
+        <v>8</v>
+      </c>
+      <c r="D70" s="49"/>
+      <c r="E70" s="50">
+        <v>8</v>
+      </c>
+      <c r="F70" s="50"/>
+      <c r="G70" s="51">
+        <v>7</v>
+      </c>
+      <c r="H70" s="51"/>
+      <c r="I70" s="50">
+        <v>8</v>
+      </c>
+      <c r="J70" s="50"/>
       <c r="K70" s="8"/>
       <c r="L70" s="8"/>
       <c r="M70" s="30">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="N70" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="N70" s="2"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A71" s="50"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="49"/>
-      <c r="D71" s="49"/>
-      <c r="E71" s="50"/>
-      <c r="F71" s="50"/>
-      <c r="G71" s="51"/>
-      <c r="H71" s="51"/>
-      <c r="I71" s="50"/>
-      <c r="J71" s="50"/>
+      <c r="A71" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" s="22">
+        <v>8</v>
+      </c>
+      <c r="D71" s="22"/>
+      <c r="E71" s="1">
+        <v>8</v>
+      </c>
+      <c r="F71" s="1"/>
+      <c r="G71" s="17">
+        <v>8</v>
+      </c>
+      <c r="H71" s="17"/>
+      <c r="I71" s="1">
+        <v>8</v>
+      </c>
+      <c r="J71" s="1"/>
       <c r="K71" s="8"/>
       <c r="L71" s="8"/>
-      <c r="M71" s="30"/>
-      <c r="N71" s="2"/>
+      <c r="M71" s="30">
+        <f t="shared" si="11"/>
+        <v>32</v>
+      </c>
+      <c r="N71" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>13</v>
+      <c r="A72" s="28" t="s">
+        <v>12</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C72" s="22">
-        <v>8</v>
+        <v>64</v>
+      </c>
+      <c r="C72" s="54">
+        <v>0</v>
       </c>
       <c r="D72" s="22"/>
       <c r="E72" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H72" s="17"/>
       <c r="I72" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J72" s="1"/>
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
       <c r="M72" s="30">
         <f t="shared" si="11"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="N72" s="2">
         <f t="shared" si="7"/>
@@ -3543,76 +3613,61 @@
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C73" s="22">
-        <v>8</v>
-      </c>
-      <c r="D73" s="22"/>
-      <c r="E73" s="1">
-        <v>8</v>
-      </c>
-      <c r="F73" s="1"/>
-      <c r="G73" s="17">
-        <v>8</v>
-      </c>
-      <c r="H73" s="17"/>
-      <c r="I73" s="1">
-        <v>7</v>
-      </c>
-      <c r="J73" s="1"/>
+      <c r="A73" s="50"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="49"/>
+      <c r="E73" s="50"/>
+      <c r="F73" s="50"/>
+      <c r="G73" s="51"/>
+      <c r="H73" s="51"/>
+      <c r="I73" s="50"/>
+      <c r="J73" s="50"/>
       <c r="K73" s="8"/>
       <c r="L73" s="8"/>
-      <c r="M73" s="30">
-        <f t="shared" si="11"/>
-        <v>31</v>
-      </c>
-      <c r="N73" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="M73" s="30"/>
+      <c r="N73" s="2"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A74" s="50" t="s">
+      <c r="A74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C74" s="49">
-        <v>0</v>
-      </c>
-      <c r="D74" s="49"/>
-      <c r="E74" s="50">
-        <v>0</v>
-      </c>
-      <c r="F74" s="50"/>
-      <c r="G74" s="51">
-        <v>0</v>
-      </c>
-      <c r="H74" s="51"/>
-      <c r="I74" s="50">
-        <v>1</v>
-      </c>
-      <c r="J74" s="50"/>
+      <c r="B74" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C74" s="22">
+        <v>8</v>
+      </c>
+      <c r="D74" s="22"/>
+      <c r="E74" s="1">
+        <v>8</v>
+      </c>
+      <c r="F74" s="1"/>
+      <c r="G74" s="17">
+        <v>8</v>
+      </c>
+      <c r="H74" s="17"/>
+      <c r="I74" s="1">
+        <v>8</v>
+      </c>
+      <c r="J74" s="1"/>
       <c r="K74" s="8"/>
       <c r="L74" s="8"/>
       <c r="M74" s="30">
         <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="N74" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="N74" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B75" s="13" t="s">
-        <v>53</v>
+      <c r="B75" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="C75" s="22">
         <v>8</v>
@@ -3627,14 +3682,14 @@
       </c>
       <c r="H75" s="17"/>
       <c r="I75" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="8"/>
       <c r="L75" s="8"/>
       <c r="M75" s="30">
         <f t="shared" si="11"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N75" s="2">
         <f t="shared" si="7"/>
@@ -3642,45 +3697,42 @@
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A76" s="28" t="s">
+      <c r="A76" s="50" t="s">
         <v>13</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C76" s="22">
-        <v>8</v>
-      </c>
-      <c r="D76" s="22"/>
-      <c r="E76" s="1">
-        <v>8</v>
-      </c>
-      <c r="F76" s="1"/>
-      <c r="G76" s="17">
-        <v>8</v>
-      </c>
-      <c r="H76" s="17"/>
-      <c r="I76" s="1">
-        <v>8</v>
-      </c>
-      <c r="J76" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="C76" s="49">
+        <v>0</v>
+      </c>
+      <c r="D76" s="49"/>
+      <c r="E76" s="50">
+        <v>0</v>
+      </c>
+      <c r="F76" s="50"/>
+      <c r="G76" s="51">
+        <v>0</v>
+      </c>
+      <c r="H76" s="51"/>
+      <c r="I76" s="50">
+        <v>1</v>
+      </c>
+      <c r="J76" s="50"/>
       <c r="K76" s="8"/>
       <c r="L76" s="8"/>
       <c r="M76" s="30">
         <f t="shared" si="11"/>
-        <v>32</v>
-      </c>
-      <c r="N76" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="N76" s="2"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B77" s="12" t="s">
-        <v>52</v>
+      <c r="B77" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="C77" s="22">
         <v>8</v>
@@ -3713,114 +3765,182 @@
       <c r="A78" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B78" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C78" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="D78" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="E78" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F78" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G78" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="H78" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="I78" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="J78" s="38" t="s">
-        <v>17</v>
-      </c>
+      <c r="B78" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C78" s="22">
+        <v>8</v>
+      </c>
+      <c r="D78" s="22"/>
+      <c r="E78" s="1">
+        <v>8</v>
+      </c>
+      <c r="F78" s="1"/>
+      <c r="G78" s="17">
+        <v>8</v>
+      </c>
+      <c r="H78" s="17"/>
+      <c r="I78" s="1">
+        <v>8</v>
+      </c>
+      <c r="J78" s="1"/>
       <c r="K78" s="8"/>
       <c r="L78" s="8"/>
-      <c r="M78" s="30" t="e">
+      <c r="M78" s="30">
+        <f t="shared" si="11"/>
+        <v>32</v>
+      </c>
+      <c r="N78" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C79" s="22">
+        <v>8</v>
+      </c>
+      <c r="D79" s="22"/>
+      <c r="E79" s="1">
+        <v>8</v>
+      </c>
+      <c r="F79" s="1"/>
+      <c r="G79" s="17">
+        <v>8</v>
+      </c>
+      <c r="H79" s="17"/>
+      <c r="I79" s="1">
+        <v>8</v>
+      </c>
+      <c r="J79" s="1"/>
+      <c r="K79" s="8"/>
+      <c r="L79" s="8"/>
+      <c r="M79" s="30">
+        <f t="shared" si="11"/>
+        <v>32</v>
+      </c>
+      <c r="N79" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F80" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G80" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="H80" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="I80" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J80" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K80" s="8"/>
+      <c r="L80" s="8"/>
+      <c r="M80" s="30" t="e">
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N78" s="2" t="e">
+      <c r="N80" s="2" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A79" s="10"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="18"/>
-      <c r="H79" s="18"/>
-      <c r="I79" s="10"/>
-      <c r="J79" s="10"/>
-      <c r="K79" s="8"/>
-      <c r="L79" s="8"/>
-      <c r="M79" s="31">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A81" s="10"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="10"/>
+      <c r="J81" s="10"/>
+      <c r="K81" s="8"/>
+      <c r="L81" s="8"/>
+      <c r="M81" s="31">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N79" s="11"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A80" s="32"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="34">
-        <f t="shared" ref="C80:J80" si="12">SUM(C5:C79)</f>
-        <v>133</v>
-      </c>
-      <c r="D80" s="34">
+      <c r="N81" s="11"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A82" s="32"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="34">
+        <f t="shared" ref="C82:J82" si="12">SUM(C5:C81)</f>
+        <v>135</v>
+      </c>
+      <c r="D82" s="34">
         <f t="shared" si="12"/>
-        <v>43.5</v>
-      </c>
-      <c r="E80" s="34">
+        <v>45.5</v>
+      </c>
+      <c r="E82" s="34">
         <f t="shared" si="12"/>
         <v>134</v>
       </c>
-      <c r="F80" s="34">
+      <c r="F82" s="34">
         <f t="shared" si="12"/>
         <v>41</v>
       </c>
-      <c r="G80" s="34">
+      <c r="G82" s="34">
         <f t="shared" si="12"/>
         <v>125.5</v>
       </c>
-      <c r="H80" s="34">
+      <c r="H82" s="34">
         <f t="shared" si="12"/>
         <v>40</v>
       </c>
-      <c r="I80" s="34">
+      <c r="I82" s="34">
         <f t="shared" si="12"/>
-        <v>128</v>
-      </c>
-      <c r="J80" s="34">
+        <v>130.5</v>
+      </c>
+      <c r="J82" s="34">
         <f t="shared" si="12"/>
-        <v>41</v>
-      </c>
-      <c r="K80" s="34"/>
-      <c r="L80" s="34"/>
-      <c r="M80" s="32">
-        <f>C80+E80+G80+I80+K80</f>
-        <v>520.5</v>
-      </c>
-      <c r="N80" s="34">
-        <f>D80+F80+H80+J80+L80</f>
-        <v>165.5</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B81" s="33" t="s">
+        <v>45.5</v>
+      </c>
+      <c r="K82" s="34"/>
+      <c r="L82" s="34"/>
+      <c r="M82" s="32">
+        <f>C82+E82+G82+I82+K82</f>
+        <v>525</v>
+      </c>
+      <c r="N82" s="34">
+        <f>D82+F82+H82+J82+L82</f>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B83" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="K81" s="43"/>
+      <c r="K83" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3854,7 +3974,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3868,12 +3993,7 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4038,9 +4158,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4062,9 +4182,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Urenverantwoording Eerste Project week
</commit_message>
<xml_diff>
--- a/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
+++ b/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
   <si>
     <t>Omschrijving activiteit</t>
   </si>
@@ -291,12 +291,6 @@
     <t>Dag 2 Doxygen testen</t>
   </si>
   <si>
-    <t>Dag 5 Maken wasprogramma uitvoeren</t>
-  </si>
-  <si>
-    <t>Dag 5 Code optimaliseren/ bug fixen / uitlopen / extra tijd</t>
-  </si>
-  <si>
     <t>Dag 1 Code optimaliseren/ bug fixen / uitlopen / extra tijd</t>
   </si>
   <si>
@@ -397,6 +391,9 @@
   <si>
     <t>Dag 4 Code maken</t>
   </si>
+  <si>
+    <t>Dag 5 Werken aan code en HTML website</t>
+  </si>
 </sst>
 </file>
 
@@ -405,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -445,12 +442,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -569,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,9 +691,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1082,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N86"/>
+  <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1125,24 +1113,24 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="78" t="s">
+      <c r="D3" s="76"/>
+      <c r="E3" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="79" t="s">
+      <c r="F3" s="77"/>
+      <c r="G3" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="78" t="s">
+      <c r="H3" s="78"/>
+      <c r="I3" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="78"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="76"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="75"/>
       <c r="M3" s="26" t="s">
         <v>9</v>
       </c>
@@ -1318,11 +1306,11 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="64">
+      <c r="A8" s="63">
         <v>1</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="20">
         <v>0</v>
@@ -1630,11 +1618,11 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="64">
+      <c r="A16" s="63">
         <v>2</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="20">
         <v>0</v>
@@ -2154,7 +2142,7 @@
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="30">
-        <f t="shared" ref="M29:N83" si="7">C29+E29+G29+I29+K29</f>
+        <f t="shared" ref="M29:N82" si="7">C29+E29+G29+I29+K29</f>
         <v>6</v>
       </c>
       <c r="N29" s="2">
@@ -2335,7 +2323,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C34" s="21">
         <v>3</v>
@@ -2350,7 +2338,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H34" s="16">
         <v>3.5</v>
@@ -2376,28 +2364,28 @@
       <c r="B35" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="55" t="s">
+      <c r="C35" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="55" t="s">
+      <c r="D35" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="56" t="s">
+      <c r="E35" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="56" t="s">
+      <c r="F35" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="57" t="s">
+      <c r="G35" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="H35" s="57" t="s">
+      <c r="H35" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="I35" s="56" t="s">
+      <c r="I35" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="56" t="s">
+      <c r="J35" s="55" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="8"/>
@@ -2418,28 +2406,28 @@
       <c r="B36" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="55" t="s">
+      <c r="C36" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="55" t="s">
+      <c r="D36" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="56" t="s">
+      <c r="E36" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="56" t="s">
+      <c r="F36" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G36" s="57" t="s">
+      <c r="G36" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="H36" s="57" t="s">
+      <c r="H36" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="I36" s="56" t="s">
+      <c r="I36" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="J36" s="56" t="s">
+      <c r="J36" s="55" t="s">
         <v>17</v>
       </c>
       <c r="K36" s="8"/>
@@ -2474,7 +2462,7 @@
         <v>5</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C38" s="21">
         <v>2</v>
@@ -2516,7 +2504,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C39" s="21">
         <v>1</v>
@@ -2594,7 +2582,7 @@
         <v>5</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C41" s="21">
         <v>0.5</v>
@@ -2636,7 +2624,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C42" s="21">
         <v>1.5</v>
@@ -2678,7 +2666,7 @@
         <v>5</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C43" s="21">
         <v>0.5</v>
@@ -2716,11 +2704,11 @@
       </c>
     </row>
     <row r="44" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="64">
+      <c r="A44" s="63">
         <v>5</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C44" s="21">
         <v>0</v>
@@ -2781,7 +2769,7 @@
         <v>6</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C46" s="49">
         <v>0</v>
@@ -2849,34 +2837,34 @@
       <c r="N47" s="2"/>
     </row>
     <row r="48" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="64">
+      <c r="A48" s="63">
         <v>6</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="63">
-        <v>0</v>
-      </c>
-      <c r="D48" s="63">
-        <v>0</v>
-      </c>
-      <c r="E48" s="64">
-        <v>0</v>
-      </c>
-      <c r="F48" s="64">
-        <v>0</v>
-      </c>
-      <c r="G48" s="65">
-        <v>0</v>
-      </c>
-      <c r="H48" s="65">
-        <v>0</v>
-      </c>
-      <c r="I48" s="64">
+        <v>69</v>
+      </c>
+      <c r="C48" s="62">
+        <v>0</v>
+      </c>
+      <c r="D48" s="62">
+        <v>0</v>
+      </c>
+      <c r="E48" s="63">
+        <v>0</v>
+      </c>
+      <c r="F48" s="63">
+        <v>0</v>
+      </c>
+      <c r="G48" s="64">
+        <v>0</v>
+      </c>
+      <c r="H48" s="64">
+        <v>0</v>
+      </c>
+      <c r="I48" s="63">
         <v>1.5</v>
       </c>
-      <c r="J48" s="64">
+      <c r="J48" s="63">
         <v>1.5</v>
       </c>
       <c r="K48" s="8"/>
@@ -2889,7 +2877,7 @@
         <v>6</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C49" s="49">
         <v>0.5</v>
@@ -2925,7 +2913,7 @@
         <v>6</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C50" s="22">
         <v>0.5</v>
@@ -2963,34 +2951,34 @@
       </c>
     </row>
     <row r="51" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="61">
+      <c r="A51" s="60">
         <v>6</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" s="60">
-        <v>2</v>
-      </c>
-      <c r="D51" s="60">
-        <v>1</v>
-      </c>
-      <c r="E51" s="61">
-        <v>2</v>
-      </c>
-      <c r="F51" s="61">
-        <v>1</v>
-      </c>
-      <c r="G51" s="62">
-        <v>0</v>
-      </c>
-      <c r="H51" s="62">
-        <v>0</v>
-      </c>
-      <c r="I51" s="61">
-        <v>2</v>
-      </c>
-      <c r="J51" s="61">
+        <v>60</v>
+      </c>
+      <c r="C51" s="59">
+        <v>2</v>
+      </c>
+      <c r="D51" s="59">
+        <v>1</v>
+      </c>
+      <c r="E51" s="60">
+        <v>2</v>
+      </c>
+      <c r="F51" s="60">
+        <v>1</v>
+      </c>
+      <c r="G51" s="61">
+        <v>0</v>
+      </c>
+      <c r="H51" s="61">
+        <v>0</v>
+      </c>
+      <c r="I51" s="60">
+        <v>2</v>
+      </c>
+      <c r="J51" s="60">
         <v>1</v>
       </c>
       <c r="K51" s="8"/>
@@ -3029,10 +3017,10 @@
       <c r="B53" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="58" t="s">
+      <c r="C53" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="D53" s="58" t="s">
+      <c r="D53" s="57" t="s">
         <v>17</v>
       </c>
       <c r="E53" s="38" t="s">
@@ -3041,10 +3029,10 @@
       <c r="F53" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="G53" s="59" t="s">
+      <c r="G53" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="H53" s="59" t="s">
+      <c r="H53" s="58" t="s">
         <v>17</v>
       </c>
       <c r="I53" s="38" t="s">
@@ -3141,7 +3129,7 @@
         <v>22</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C56" s="39">
         <v>4</v>
@@ -3233,34 +3221,34 @@
       <c r="N59" s="2"/>
     </row>
     <row r="60" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="67" t="s">
-        <v>73</v>
+      <c r="A60" s="66" t="s">
+        <v>71</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C60" s="66">
-        <v>2</v>
-      </c>
-      <c r="D60" s="66">
-        <v>2</v>
-      </c>
-      <c r="E60" s="67">
-        <v>0</v>
-      </c>
-      <c r="F60" s="67">
-        <v>0</v>
-      </c>
-      <c r="G60" s="68">
-        <v>0</v>
-      </c>
-      <c r="H60" s="68">
-        <v>0</v>
-      </c>
-      <c r="I60" s="67">
+        <v>72</v>
+      </c>
+      <c r="C60" s="65">
+        <v>2</v>
+      </c>
+      <c r="D60" s="65">
+        <v>2</v>
+      </c>
+      <c r="E60" s="66">
+        <v>0</v>
+      </c>
+      <c r="F60" s="66">
+        <v>0</v>
+      </c>
+      <c r="G60" s="67">
+        <v>0</v>
+      </c>
+      <c r="H60" s="67">
+        <v>0</v>
+      </c>
+      <c r="I60" s="66">
         <v>1.5</v>
       </c>
-      <c r="J60" s="67">
+      <c r="J60" s="66">
         <v>1.5</v>
       </c>
       <c r="K60" s="8"/>
@@ -3269,34 +3257,34 @@
       <c r="N60" s="2"/>
     </row>
     <row r="61" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="67" t="s">
+      <c r="A61" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C61" s="66">
-        <v>0</v>
-      </c>
-      <c r="D61" s="66">
-        <v>0</v>
-      </c>
-      <c r="E61" s="67">
-        <v>0</v>
-      </c>
-      <c r="F61" s="67">
-        <v>0</v>
-      </c>
-      <c r="G61" s="68">
-        <v>0</v>
-      </c>
-      <c r="H61" s="68">
-        <v>0</v>
-      </c>
-      <c r="I61" s="67">
-        <v>1</v>
-      </c>
-      <c r="J61" s="67">
+      <c r="C61" s="65">
+        <v>0</v>
+      </c>
+      <c r="D61" s="65">
+        <v>0</v>
+      </c>
+      <c r="E61" s="66">
+        <v>0</v>
+      </c>
+      <c r="F61" s="66">
+        <v>0</v>
+      </c>
+      <c r="G61" s="67">
+        <v>0</v>
+      </c>
+      <c r="H61" s="67">
+        <v>0</v>
+      </c>
+      <c r="I61" s="66">
+        <v>1</v>
+      </c>
+      <c r="J61" s="66">
         <v>1</v>
       </c>
       <c r="K61" s="8"/>
@@ -3325,7 +3313,7 @@
         <v>12</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C63" s="22">
         <v>3</v>
@@ -3367,7 +3355,7 @@
         <v>12</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C64" s="22">
         <v>1.5</v>
@@ -3409,7 +3397,7 @@
         <v>12</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C65" s="49">
         <v>1</v>
@@ -3441,34 +3429,34 @@
       <c r="N65" s="2"/>
     </row>
     <row r="66" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="70" t="s">
+      <c r="A66" s="69" t="s">
         <v>12</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C66" s="69">
-        <v>2</v>
-      </c>
-      <c r="D66" s="69">
-        <v>2</v>
-      </c>
-      <c r="E66" s="70">
-        <v>2</v>
-      </c>
-      <c r="F66" s="70">
-        <v>2</v>
-      </c>
-      <c r="G66" s="71">
-        <v>0</v>
-      </c>
-      <c r="H66" s="71">
-        <v>0</v>
-      </c>
-      <c r="I66" s="70">
-        <v>0</v>
-      </c>
-      <c r="J66" s="70">
+        <v>78</v>
+      </c>
+      <c r="C66" s="68">
+        <v>2</v>
+      </c>
+      <c r="D66" s="68">
+        <v>2</v>
+      </c>
+      <c r="E66" s="69">
+        <v>2</v>
+      </c>
+      <c r="F66" s="69">
+        <v>2</v>
+      </c>
+      <c r="G66" s="70">
+        <v>0</v>
+      </c>
+      <c r="H66" s="70">
+        <v>0</v>
+      </c>
+      <c r="I66" s="69">
+        <v>0</v>
+      </c>
+      <c r="J66" s="69">
         <v>0</v>
       </c>
       <c r="K66" s="8"/>
@@ -3481,7 +3469,7 @@
         <v>12</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C67" s="49">
         <v>2</v>
@@ -3517,7 +3505,7 @@
         <v>12</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C68" s="22">
         <v>0.5</v>
@@ -3559,7 +3547,7 @@
         <v>12</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C69" s="49">
         <v>2</v>
@@ -3591,34 +3579,34 @@
       <c r="N69" s="2"/>
     </row>
     <row r="70" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="73" t="s">
+      <c r="A70" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" s="72">
-        <v>2</v>
-      </c>
-      <c r="D70" s="72">
-        <v>2</v>
-      </c>
-      <c r="E70" s="73">
-        <v>2</v>
-      </c>
-      <c r="F70" s="73">
-        <v>2</v>
-      </c>
-      <c r="G70" s="74">
-        <v>0</v>
-      </c>
-      <c r="H70" s="74">
-        <v>0</v>
-      </c>
-      <c r="I70" s="73">
-        <v>0</v>
-      </c>
-      <c r="J70" s="73">
+        <v>81</v>
+      </c>
+      <c r="C70" s="71">
+        <v>2</v>
+      </c>
+      <c r="D70" s="71">
+        <v>2</v>
+      </c>
+      <c r="E70" s="72">
+        <v>2</v>
+      </c>
+      <c r="F70" s="72">
+        <v>2</v>
+      </c>
+      <c r="G70" s="73">
+        <v>0</v>
+      </c>
+      <c r="H70" s="73">
+        <v>0</v>
+      </c>
+      <c r="I70" s="72">
+        <v>0</v>
+      </c>
+      <c r="J70" s="72">
         <v>0</v>
       </c>
       <c r="K70" s="8"/>
@@ -3627,34 +3615,34 @@
       <c r="N70" s="2"/>
     </row>
     <row r="71" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="73" t="s">
+      <c r="A71" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C71" s="72">
-        <v>0</v>
-      </c>
-      <c r="D71" s="72">
-        <v>0</v>
-      </c>
-      <c r="E71" s="73">
-        <v>0</v>
-      </c>
-      <c r="F71" s="73">
-        <v>0</v>
-      </c>
-      <c r="G71" s="74">
-        <v>2</v>
-      </c>
-      <c r="H71" s="74">
-        <v>2</v>
-      </c>
-      <c r="I71" s="73">
-        <v>2</v>
-      </c>
-      <c r="J71" s="73">
+        <v>82</v>
+      </c>
+      <c r="C71" s="71">
+        <v>0</v>
+      </c>
+      <c r="D71" s="71">
+        <v>0</v>
+      </c>
+      <c r="E71" s="72">
+        <v>0</v>
+      </c>
+      <c r="F71" s="72">
+        <v>0</v>
+      </c>
+      <c r="G71" s="73">
+        <v>2</v>
+      </c>
+      <c r="H71" s="73">
+        <v>0</v>
+      </c>
+      <c r="I71" s="72">
+        <v>2</v>
+      </c>
+      <c r="J71" s="72">
         <v>2</v>
       </c>
       <c r="K71" s="8"/>
@@ -3667,7 +3655,7 @@
         <v>12</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C72" s="22">
         <v>6</v>
@@ -3696,7 +3684,7 @@
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
       <c r="M72" s="30">
-        <f t="shared" ref="M72:M84" si="11">C72+E72+G72+I72+K72</f>
+        <f t="shared" ref="M72:M83" si="11">C72+E72+G72+I72+K72</f>
         <v>12</v>
       </c>
       <c r="N72" s="2">
@@ -3709,7 +3697,7 @@
         <v>12</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C73" s="49">
         <v>0</v>
@@ -3748,91 +3736,101 @@
         <v>12</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="C74" s="22">
-        <v>8</v>
-      </c>
-      <c r="D74" s="22"/>
+        <v>6</v>
+      </c>
+      <c r="D74" s="22">
+        <v>6</v>
+      </c>
       <c r="E74" s="1">
-        <v>8</v>
-      </c>
-      <c r="F74" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F74" s="1">
+        <v>6</v>
+      </c>
       <c r="G74" s="17">
-        <v>8</v>
-      </c>
-      <c r="H74" s="17"/>
+        <v>0</v>
+      </c>
+      <c r="H74" s="17">
+        <v>0</v>
+      </c>
       <c r="I74" s="1">
-        <v>8</v>
-      </c>
-      <c r="J74" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="J74" s="1">
+        <v>6</v>
+      </c>
       <c r="K74" s="8"/>
       <c r="L74" s="8"/>
       <c r="M74" s="30">
         <f t="shared" si="11"/>
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="N74" s="2">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A75" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C75" s="54">
-        <v>0</v>
-      </c>
-      <c r="D75" s="22"/>
-      <c r="E75" s="1">
-        <v>0</v>
-      </c>
-      <c r="F75" s="1"/>
-      <c r="G75" s="17">
-        <v>0</v>
-      </c>
-      <c r="H75" s="17"/>
-      <c r="I75" s="1">
-        <v>0</v>
-      </c>
-      <c r="J75" s="1"/>
+      <c r="A75" s="50"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="49"/>
+      <c r="D75" s="49"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="51"/>
+      <c r="H75" s="51"/>
+      <c r="I75" s="50"/>
+      <c r="J75" s="50"/>
       <c r="K75" s="8"/>
       <c r="L75" s="8"/>
-      <c r="M75" s="30">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="N75" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+      <c r="M75" s="30"/>
+      <c r="N75" s="2"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A76" s="50"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
-      <c r="E76" s="50"/>
-      <c r="F76" s="50"/>
-      <c r="G76" s="51"/>
-      <c r="H76" s="51"/>
-      <c r="I76" s="50"/>
-      <c r="J76" s="50"/>
+      <c r="A76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" s="22">
+        <v>8</v>
+      </c>
+      <c r="D76" s="22"/>
+      <c r="E76" s="1">
+        <v>8</v>
+      </c>
+      <c r="F76" s="1"/>
+      <c r="G76" s="17">
+        <v>0</v>
+      </c>
+      <c r="H76" s="17">
+        <v>0</v>
+      </c>
+      <c r="I76" s="1">
+        <v>8</v>
+      </c>
+      <c r="J76" s="1"/>
       <c r="K76" s="8"/>
       <c r="L76" s="8"/>
-      <c r="M76" s="30"/>
-      <c r="N76" s="2"/>
+      <c r="M76" s="30">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="N76" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B77" s="13" t="s">
-        <v>57</v>
+      <c r="B77" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="C77" s="22">
         <v>8</v>
@@ -3843,18 +3841,20 @@
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="17">
-        <v>8</v>
-      </c>
-      <c r="H77" s="17"/>
+        <v>0</v>
+      </c>
+      <c r="H77" s="17">
+        <v>0</v>
+      </c>
       <c r="I77" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J77" s="1"/>
       <c r="K77" s="8"/>
       <c r="L77" s="8"/>
       <c r="M77" s="30">
         <f t="shared" si="11"/>
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="N77" s="2">
         <f t="shared" si="7"/>
@@ -3862,76 +3862,80 @@
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A78" s="28" t="s">
+      <c r="A78" s="50" t="s">
         <v>13</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C78" s="22">
-        <v>8</v>
-      </c>
-      <c r="D78" s="22"/>
-      <c r="E78" s="1">
-        <v>8</v>
-      </c>
-      <c r="F78" s="1"/>
-      <c r="G78" s="17">
-        <v>8</v>
-      </c>
-      <c r="H78" s="17"/>
-      <c r="I78" s="1">
-        <v>7</v>
-      </c>
-      <c r="J78" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="C78" s="49">
+        <v>0</v>
+      </c>
+      <c r="D78" s="49"/>
+      <c r="E78" s="50">
+        <v>0</v>
+      </c>
+      <c r="F78" s="50"/>
+      <c r="G78" s="51">
+        <v>0</v>
+      </c>
+      <c r="H78" s="51">
+        <v>0</v>
+      </c>
+      <c r="I78" s="50">
+        <v>1</v>
+      </c>
+      <c r="J78" s="50"/>
       <c r="K78" s="8"/>
       <c r="L78" s="8"/>
       <c r="M78" s="30">
         <f t="shared" si="11"/>
-        <v>31</v>
-      </c>
-      <c r="N78" s="2">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="N78" s="2"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A79" s="50" t="s">
+      <c r="A79" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B79" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C79" s="49">
-        <v>0</v>
-      </c>
-      <c r="D79" s="49"/>
-      <c r="E79" s="50">
-        <v>0</v>
-      </c>
-      <c r="F79" s="50"/>
-      <c r="G79" s="51">
-        <v>0</v>
-      </c>
-      <c r="H79" s="51"/>
-      <c r="I79" s="50">
-        <v>1</v>
-      </c>
-      <c r="J79" s="50"/>
+      <c r="B79" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="22">
+        <v>8</v>
+      </c>
+      <c r="D79" s="22"/>
+      <c r="E79" s="1">
+        <v>8</v>
+      </c>
+      <c r="F79" s="1"/>
+      <c r="G79" s="17">
+        <v>0</v>
+      </c>
+      <c r="H79" s="17">
+        <v>0</v>
+      </c>
+      <c r="I79" s="1">
+        <v>8</v>
+      </c>
+      <c r="J79" s="1"/>
       <c r="K79" s="8"/>
       <c r="L79" s="8"/>
       <c r="M79" s="30">
         <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="N79" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="N79" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B80" s="13" t="s">
-        <v>51</v>
+      <c r="B80" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="C80" s="22">
         <v>8</v>
@@ -3942,9 +3946,11 @@
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="17">
-        <v>8</v>
-      </c>
-      <c r="H80" s="17"/>
+        <v>0</v>
+      </c>
+      <c r="H80" s="17">
+        <v>0</v>
+      </c>
       <c r="I80" s="1">
         <v>8</v>
       </c>
@@ -3953,7 +3959,7 @@
       <c r="L80" s="8"/>
       <c r="M80" s="30">
         <f t="shared" si="11"/>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="N80" s="2">
         <f t="shared" si="7"/>
@@ -3965,7 +3971,7 @@
         <v>13</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C81" s="22">
         <v>8</v>
@@ -3976,9 +3982,11 @@
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="17">
-        <v>8</v>
-      </c>
-      <c r="H81" s="17"/>
+        <v>0</v>
+      </c>
+      <c r="H81" s="17">
+        <v>0</v>
+      </c>
       <c r="I81" s="1">
         <v>8</v>
       </c>
@@ -3987,7 +3995,7 @@
       <c r="L81" s="8"/>
       <c r="M81" s="30">
         <f t="shared" si="11"/>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="N81" s="2">
         <f t="shared" si="7"/>
@@ -3998,148 +4006,114 @@
       <c r="A82" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B82" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C82" s="22">
-        <v>8</v>
-      </c>
-      <c r="D82" s="22"/>
-      <c r="E82" s="1">
-        <v>8</v>
-      </c>
-      <c r="F82" s="1"/>
-      <c r="G82" s="17">
-        <v>8</v>
-      </c>
-      <c r="H82" s="17"/>
-      <c r="I82" s="1">
-        <v>8</v>
-      </c>
-      <c r="J82" s="1"/>
+      <c r="B82" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C82" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E82" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F82" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G82" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H82" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="I82" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J82" s="38" t="s">
+        <v>17</v>
+      </c>
       <c r="K82" s="8"/>
       <c r="L82" s="8"/>
-      <c r="M82" s="30">
+      <c r="M82" s="30" t="e">
         <f t="shared" si="11"/>
-        <v>32</v>
-      </c>
-      <c r="N82" s="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N82" s="2" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A83" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B83" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C83" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="D83" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="E83" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F83" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G83" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="H83" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="I83" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="J83" s="38" t="s">
-        <v>17</v>
-      </c>
+      <c r="A83" s="10"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="10"/>
       <c r="K83" s="8"/>
       <c r="L83" s="8"/>
-      <c r="M83" s="30" t="e">
+      <c r="M83" s="31">
         <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N83" s="2" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N83" s="11"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A84" s="10"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="23"/>
-      <c r="D84" s="23"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="10"/>
-      <c r="G84" s="18"/>
-      <c r="H84" s="18"/>
-      <c r="I84" s="10"/>
-      <c r="J84" s="10"/>
-      <c r="K84" s="8"/>
-      <c r="L84" s="8"/>
-      <c r="M84" s="31">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="N84" s="11"/>
+      <c r="A84" s="32"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="34">
+        <f t="shared" ref="C84:J84" si="12">SUM(C5:C83)</f>
+        <v>121</v>
+      </c>
+      <c r="D84" s="34">
+        <f t="shared" si="12"/>
+        <v>71.5</v>
+      </c>
+      <c r="E84" s="34">
+        <f t="shared" si="12"/>
+        <v>120</v>
+      </c>
+      <c r="F84" s="34">
+        <f t="shared" si="12"/>
+        <v>68.5</v>
+      </c>
+      <c r="G84" s="34">
+        <f t="shared" si="12"/>
+        <v>63.5</v>
+      </c>
+      <c r="H84" s="34">
+        <f t="shared" si="12"/>
+        <v>48</v>
+      </c>
+      <c r="I84" s="34">
+        <f t="shared" si="12"/>
+        <v>112</v>
+      </c>
+      <c r="J84" s="34">
+        <f t="shared" si="12"/>
+        <v>64.5</v>
+      </c>
+      <c r="K84" s="34"/>
+      <c r="L84" s="34"/>
+      <c r="M84" s="32">
+        <f>C84+E84+G84+I84+K84</f>
+        <v>416.5</v>
+      </c>
+      <c r="N84" s="34">
+        <f>D84+F84+H84+J84+L84</f>
+        <v>252.5</v>
+      </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A85" s="32"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="34">
-        <f t="shared" ref="C85:J85" si="12">SUM(C5:C84)</f>
-        <v>123</v>
-      </c>
-      <c r="D85" s="34">
-        <f t="shared" si="12"/>
-        <v>65.5</v>
-      </c>
-      <c r="E85" s="34">
-        <f t="shared" si="12"/>
-        <v>122</v>
-      </c>
-      <c r="F85" s="34">
-        <f t="shared" si="12"/>
-        <v>62.5</v>
-      </c>
-      <c r="G85" s="34">
-        <f t="shared" si="12"/>
-        <v>111.5</v>
-      </c>
-      <c r="H85" s="34">
-        <f t="shared" si="12"/>
-        <v>50</v>
-      </c>
-      <c r="I85" s="34">
-        <f t="shared" si="12"/>
-        <v>114</v>
-      </c>
-      <c r="J85" s="34">
-        <f t="shared" si="12"/>
-        <v>58.5</v>
-      </c>
-      <c r="K85" s="34"/>
-      <c r="L85" s="34"/>
-      <c r="M85" s="32">
-        <f>C85+E85+G85+I85+K85</f>
-        <v>470.5</v>
-      </c>
-      <c r="N85" s="34">
-        <f>D85+F85+H85+J85+L85</f>
-        <v>236.5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B86" s="33" t="s">
+      <c r="B85" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="K86" s="43"/>
+      <c r="K85" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4173,25 +4147,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
-    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
-    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D777D35650D3B43A23D41664AA30BC5" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="7f80e5700d93aba1c148b391c267eb5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ab5e87a-ed8e-45a5-9793-059f67398425" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e36a552b910c1cdf142adc90bba5ebe9" ns2:_="">
     <xsd:import namespace="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
@@ -4352,35 +4311,34 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
+    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
+    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6B4BC2B-47EC-4A4E-997D-A663CFE6E409}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4398,10 +4356,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UserInteractionTask Update en Urenverantwoording
</commit_message>
<xml_diff>
--- a/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
+++ b/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="94">
   <si>
     <t>Omschrijving activiteit</t>
   </si>
@@ -404,7 +404,19 @@
     <t>Techinisch verslag afmaken</t>
   </si>
   <si>
-    <t>Precentatie maken</t>
+    <t>Techninisch verslag afmaken</t>
+  </si>
+  <si>
+    <t>SA afmaken Verslag afmaken Presentatie maken</t>
+  </si>
+  <si>
+    <t>Overleg project afronding en Verwerken Feedback modellen</t>
+  </si>
+  <si>
+    <t>Verbeteren Std modellen</t>
+  </si>
+  <si>
+    <t>Werken aan de code en Pi</t>
   </si>
 </sst>
 </file>
@@ -572,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -772,6 +784,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -785,6 +800,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1091,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N88"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N90" sqref="N90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1134,24 +1152,24 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="80" t="s">
+      <c r="D3" s="80"/>
+      <c r="E3" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="80"/>
-      <c r="G3" s="81" t="s">
+      <c r="F3" s="81"/>
+      <c r="G3" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="81"/>
-      <c r="I3" s="80" t="s">
+      <c r="H3" s="82"/>
+      <c r="I3" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="80"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="78"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="79"/>
       <c r="M3" s="26" t="s">
         <v>9</v>
       </c>
@@ -1897,7 +1915,9 @@
       </c>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="30"/>
+      <c r="M22" s="30">
+        <v>8</v>
+      </c>
       <c r="N22" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -2163,7 +2183,7 @@
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="30">
-        <f t="shared" ref="M29:N85" si="7">C29+E29+G29+I29+K29</f>
+        <f t="shared" ref="M29:N84" si="7">C29+E29+G29+I29+K29</f>
         <v>6</v>
       </c>
       <c r="N29" s="2">
@@ -2557,7 +2577,9 @@
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="N39" s="2"/>
+      <c r="N39" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="40" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="50">
@@ -2596,7 +2618,9 @@
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="N40" s="2"/>
+      <c r="N40" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="25">
@@ -2761,7 +2785,9 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N44" s="2"/>
+      <c r="N44" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
@@ -2818,8 +2844,12 @@
       </c>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
-      <c r="M46" s="30"/>
-      <c r="N46" s="2"/>
+      <c r="M46" s="30">
+        <v>7</v>
+      </c>
+      <c r="N46" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="47" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="50">
@@ -2854,8 +2884,12 @@
       </c>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="2"/>
+      <c r="M47" s="30">
+        <v>7</v>
+      </c>
+      <c r="N47" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="48" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="63">
@@ -2890,8 +2924,12 @@
       </c>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="2"/>
+      <c r="M48" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="N48" s="2">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="49" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="50">
@@ -2926,8 +2964,12 @@
       </c>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
-      <c r="M49" s="30"/>
-      <c r="N49" s="2"/>
+      <c r="M49" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="N49" s="2">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="50" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
@@ -3705,7 +3747,7 @@
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
       <c r="M72" s="30">
-        <f t="shared" ref="M72:M86" si="11">C72+E72+G72+I72+K72</f>
+        <f t="shared" ref="M72:M89" si="11">C72+E72+G72+I72+K72</f>
         <v>12</v>
       </c>
       <c r="N72" s="2">
@@ -3839,7 +3881,7 @@
         <v>8</v>
       </c>
       <c r="J76" s="1">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="K76" s="8"/>
       <c r="L76" s="8"/>
@@ -3849,7 +3891,7 @@
       </c>
       <c r="N76" s="2">
         <f t="shared" si="7"/>
-        <v>21.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -4025,16 +4067,20 @@
         <v>84</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C81" s="74">
         <v>6</v>
       </c>
-      <c r="D81" s="74"/>
+      <c r="D81" s="74">
+        <v>4</v>
+      </c>
       <c r="E81" s="75">
-        <v>6</v>
-      </c>
-      <c r="F81" s="75"/>
+        <v>0</v>
+      </c>
+      <c r="F81" s="75">
+        <v>0</v>
+      </c>
       <c r="G81" s="76">
         <v>0</v>
       </c>
@@ -4051,9 +4097,12 @@
       <c r="L81" s="8"/>
       <c r="M81" s="30">
         <f t="shared" si="11"/>
-        <v>12</v>
-      </c>
-      <c r="N81" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="N81" s="2">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="75" t="s">
@@ -4071,7 +4120,9 @@
       <c r="E82" s="75">
         <v>6</v>
       </c>
-      <c r="F82" s="75"/>
+      <c r="F82" s="75">
+        <v>4</v>
+      </c>
       <c r="G82" s="76">
         <v>0</v>
       </c>
@@ -4081,7 +4132,9 @@
       <c r="I82" s="75">
         <v>6</v>
       </c>
-      <c r="J82" s="75"/>
+      <c r="J82" s="75">
+        <v>4</v>
+      </c>
       <c r="K82" s="8"/>
       <c r="L82" s="8"/>
       <c r="M82" s="30">
@@ -4095,16 +4148,20 @@
         <v>83</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C83" s="74">
         <v>8</v>
       </c>
-      <c r="D83" s="74"/>
+      <c r="D83" s="74">
+        <v>8</v>
+      </c>
       <c r="E83" s="75">
         <v>8</v>
       </c>
-      <c r="F83" s="75"/>
+      <c r="F83" s="75">
+        <v>8</v>
+      </c>
       <c r="G83" s="76">
         <v>0</v>
       </c>
@@ -4114,7 +4171,9 @@
       <c r="I83" s="75">
         <v>8</v>
       </c>
-      <c r="J83" s="75"/>
+      <c r="J83" s="75">
+        <v>8</v>
+      </c>
       <c r="K83" s="8"/>
       <c r="L83" s="8"/>
       <c r="M83" s="30">
@@ -4124,154 +4183,237 @@
       <c r="N83" s="2"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A84" s="75" t="s">
+      <c r="A84" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B84" s="12"/>
-      <c r="C84" s="74">
-        <v>0</v>
-      </c>
-      <c r="D84" s="74">
-        <v>0</v>
-      </c>
-      <c r="E84" s="75">
-        <v>0</v>
-      </c>
-      <c r="F84" s="75">
-        <v>0</v>
-      </c>
-      <c r="G84" s="76">
-        <v>0</v>
-      </c>
-      <c r="H84" s="76">
-        <v>0</v>
-      </c>
-      <c r="I84" s="75">
-        <v>0</v>
-      </c>
-      <c r="J84" s="75">
-        <v>0</v>
+      <c r="B84" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C84" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D84" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F84" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G84" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H84" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="I84" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J84" s="38" t="s">
+        <v>17</v>
       </c>
       <c r="K84" s="8"/>
       <c r="L84" s="8"/>
-      <c r="M84" s="30">
+      <c r="M84" s="30" t="e">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="N84" s="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N84" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A85" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="B85" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C85" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D85" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E85" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F85" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G85" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="H85" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="I85" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="J85" s="38" t="s">
-        <v>17</v>
-      </c>
+      <c r="A85" s="77"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="57"/>
+      <c r="D85" s="57"/>
+      <c r="E85" s="38"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="58"/>
+      <c r="H85" s="58"/>
+      <c r="I85" s="38"/>
+      <c r="J85" s="38"/>
       <c r="K85" s="8"/>
       <c r="L85" s="8"/>
-      <c r="M85" s="30" t="e">
-        <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N85" s="2" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="M85" s="30"/>
+      <c r="N85" s="2"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A86" s="10"/>
-      <c r="B86" s="12"/>
-      <c r="C86" s="23"/>
-      <c r="D86" s="23"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="10"/>
-      <c r="G86" s="18"/>
-      <c r="H86" s="18"/>
-      <c r="I86" s="10"/>
-      <c r="J86" s="10"/>
+      <c r="A86" s="83">
+        <v>42406</v>
+      </c>
+      <c r="B86" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86" s="57">
+        <v>0</v>
+      </c>
+      <c r="D86" s="57">
+        <v>0</v>
+      </c>
+      <c r="E86" s="38">
+        <v>0</v>
+      </c>
+      <c r="F86" s="38">
+        <v>0</v>
+      </c>
+      <c r="G86" s="58">
+        <v>0</v>
+      </c>
+      <c r="H86" s="58">
+        <v>0</v>
+      </c>
+      <c r="I86" s="38">
+        <v>6</v>
+      </c>
+      <c r="J86" s="38">
+        <v>6</v>
+      </c>
       <c r="K86" s="8"/>
       <c r="L86" s="8"/>
-      <c r="M86" s="31">
+      <c r="M86" s="30"/>
+      <c r="N86" s="2"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A87" s="83">
+        <v>42408</v>
+      </c>
+      <c r="B87" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87" s="57">
+        <v>4</v>
+      </c>
+      <c r="D87" s="57">
+        <v>4</v>
+      </c>
+      <c r="E87" s="38">
+        <v>4</v>
+      </c>
+      <c r="F87" s="38">
+        <v>4</v>
+      </c>
+      <c r="G87" s="58">
+        <v>0</v>
+      </c>
+      <c r="H87" s="58">
+        <v>0</v>
+      </c>
+      <c r="I87" s="38">
+        <v>4</v>
+      </c>
+      <c r="J87" s="38">
+        <v>4</v>
+      </c>
+      <c r="K87" s="8"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="30"/>
+      <c r="N87" s="2"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88" s="83">
+        <v>42410</v>
+      </c>
+      <c r="B88" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C88" s="57">
+        <v>8</v>
+      </c>
+      <c r="D88" s="57">
+        <v>8</v>
+      </c>
+      <c r="E88" s="38">
+        <v>8</v>
+      </c>
+      <c r="F88" s="38">
+        <v>8</v>
+      </c>
+      <c r="G88" s="58"/>
+      <c r="H88" s="58"/>
+      <c r="I88" s="38">
+        <v>8</v>
+      </c>
+      <c r="J88" s="38">
+        <v>8</v>
+      </c>
+      <c r="K88" s="8"/>
+      <c r="L88" s="8"/>
+      <c r="M88" s="30"/>
+      <c r="N88" s="2"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89" s="10"/>
+      <c r="B89" s="12"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="10"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="8"/>
+      <c r="M89" s="31">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N86" s="11"/>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A87" s="32"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="34">
-        <f>SUM(C5:C86)</f>
-        <v>135</v>
-      </c>
-      <c r="D87" s="34">
-        <f>SUM(D5:D86)</f>
-        <v>115</v>
-      </c>
-      <c r="E87" s="34">
-        <f>SUM(E5:E86)</f>
-        <v>140</v>
-      </c>
-      <c r="F87" s="34">
-        <f>SUM(F5:F86)</f>
-        <v>112.5</v>
-      </c>
-      <c r="G87" s="34">
-        <f>SUM(G5:G86)</f>
+      <c r="N89" s="11"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A90" s="32"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="34">
+        <f t="shared" ref="C90:J90" si="12">SUM(C5:C89)</f>
+        <v>147</v>
+      </c>
+      <c r="D90" s="34">
+        <f t="shared" si="12"/>
+        <v>139</v>
+      </c>
+      <c r="E90" s="34">
+        <f t="shared" si="12"/>
+        <v>146</v>
+      </c>
+      <c r="F90" s="34">
+        <f t="shared" si="12"/>
+        <v>136.5</v>
+      </c>
+      <c r="G90" s="34">
+        <f t="shared" si="12"/>
         <v>63.5</v>
       </c>
-      <c r="H87" s="34">
-        <f>SUM(H5:H86)</f>
+      <c r="H90" s="34">
+        <f t="shared" si="12"/>
         <v>51</v>
       </c>
-      <c r="I87" s="34">
-        <f>SUM(I5:I86)</f>
-        <v>127.5</v>
-      </c>
-      <c r="J87" s="34">
-        <f>SUM(J5:J86)</f>
-        <v>103.5</v>
-      </c>
-      <c r="K87" s="34"/>
-      <c r="L87" s="34"/>
-      <c r="M87" s="32">
-        <f>C87+E87+G87+I87+K87</f>
-        <v>466</v>
-      </c>
-      <c r="N87" s="34">
-        <f>D87+F87+H87+J87+L87</f>
-        <v>382</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B88" s="33" t="s">
+      <c r="I90" s="34">
+        <f t="shared" si="12"/>
+        <v>145.5</v>
+      </c>
+      <c r="J90" s="34">
+        <f t="shared" si="12"/>
+        <v>134.5</v>
+      </c>
+      <c r="K90" s="34"/>
+      <c r="L90" s="34"/>
+      <c r="M90" s="32">
+        <f>C90+E90+G90+I90+K90</f>
+        <v>502</v>
+      </c>
+      <c r="N90" s="34">
+        <f>D90+F90+H90+J90+L90</f>
+        <v>461</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B91" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="K88" s="43"/>
+      <c r="K91" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4305,10 +4447,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D777D35650D3B43A23D41664AA30BC5" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="7f80e5700d93aba1c148b391c267eb5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ab5e87a-ed8e-45a5-9793-059f67398425" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e36a552b910c1cdf142adc90bba5ebe9" ns2:_="">
     <xsd:import namespace="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
@@ -4469,7 +4607,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4478,7 +4616,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
@@ -4488,15 +4626,11 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6B4BC2B-47EC-4A4E-997D-A663CFE6E409}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4514,7 +4648,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4522,7 +4656,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -4536,4 +4670,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update urenver. en solution acrcitecture
</commit_message>
<xml_diff>
--- a/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
+++ b/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="94">
   <si>
     <t>Omschrijving activiteit</t>
   </si>
@@ -1109,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N96"/>
+  <dimension ref="A1:N99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3747,7 +3747,7 @@
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
       <c r="M72" s="30">
-        <f t="shared" ref="M72:M94" si="11">C72+E72+G72+I72+K72</f>
+        <f t="shared" ref="M72:M97" si="11">C72+E72+G72+I72+K72</f>
         <v>12</v>
       </c>
       <c r="N72" s="2">
@@ -4446,11 +4446,15 @@
       <c r="C92" s="57">
         <v>3</v>
       </c>
-      <c r="D92" s="57"/>
+      <c r="D92" s="57">
+        <v>0</v>
+      </c>
       <c r="E92" s="38">
         <v>3</v>
       </c>
-      <c r="F92" s="38"/>
+      <c r="F92" s="38">
+        <v>0</v>
+      </c>
       <c r="G92" s="58">
         <v>0</v>
       </c>
@@ -4460,7 +4464,9 @@
       <c r="I92" s="38">
         <v>3</v>
       </c>
-      <c r="J92" s="38"/>
+      <c r="J92" s="38">
+        <v>1</v>
+      </c>
       <c r="K92" s="8"/>
       <c r="L92" s="8"/>
       <c r="M92" s="30"/>
@@ -4483,75 +4489,175 @@
       <c r="N93" s="2"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A94" s="10"/>
-      <c r="B94" s="12"/>
-      <c r="C94" s="23"/>
-      <c r="D94" s="23"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="18"/>
-      <c r="H94" s="18"/>
-      <c r="I94" s="10"/>
-      <c r="J94" s="10"/>
+      <c r="A94" s="78">
+        <v>42422</v>
+      </c>
+      <c r="B94" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C94" s="57">
+        <v>7</v>
+      </c>
+      <c r="D94" s="57">
+        <v>7</v>
+      </c>
+      <c r="E94" s="38">
+        <v>7</v>
+      </c>
+      <c r="F94" s="38">
+        <v>7</v>
+      </c>
+      <c r="G94" s="58">
+        <v>0</v>
+      </c>
+      <c r="H94" s="58">
+        <v>0</v>
+      </c>
+      <c r="I94" s="38">
+        <v>7</v>
+      </c>
+      <c r="J94" s="38">
+        <v>7</v>
+      </c>
       <c r="K94" s="8"/>
       <c r="L94" s="8"/>
-      <c r="M94" s="31">
+      <c r="M94" s="30"/>
+      <c r="N94" s="2"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95" s="78">
+        <v>42423</v>
+      </c>
+      <c r="B95" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C95" s="57">
+        <v>7</v>
+      </c>
+      <c r="D95" s="57"/>
+      <c r="E95" s="38">
+        <v>7</v>
+      </c>
+      <c r="F95" s="38"/>
+      <c r="G95" s="58">
+        <v>0</v>
+      </c>
+      <c r="H95" s="58">
+        <v>0</v>
+      </c>
+      <c r="I95" s="38">
+        <v>7</v>
+      </c>
+      <c r="J95" s="38"/>
+      <c r="K95" s="8"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="30"/>
+      <c r="N95" s="2"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96" s="78">
+        <v>42424</v>
+      </c>
+      <c r="B96" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" s="57">
+        <v>7</v>
+      </c>
+      <c r="D96" s="57"/>
+      <c r="E96" s="38">
+        <v>7</v>
+      </c>
+      <c r="F96" s="38"/>
+      <c r="G96" s="58">
+        <v>0</v>
+      </c>
+      <c r="H96" s="58">
+        <v>0</v>
+      </c>
+      <c r="I96" s="38">
+        <v>7</v>
+      </c>
+      <c r="J96" s="38"/>
+      <c r="K96" s="8"/>
+      <c r="L96" s="8"/>
+      <c r="M96" s="30"/>
+      <c r="N96" s="2"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" s="10"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="18">
+        <v>0</v>
+      </c>
+      <c r="H97" s="18">
+        <v>0</v>
+      </c>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10"/>
+      <c r="K97" s="8"/>
+      <c r="L97" s="8"/>
+      <c r="M97" s="31">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N94" s="11"/>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A95" s="32"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="34">
-        <f t="shared" ref="C95:J95" si="12">SUM(C5:C94)</f>
-        <v>160</v>
-      </c>
-      <c r="D95" s="34">
+      <c r="N97" s="11"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="32"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="34">
+        <f t="shared" ref="C98:J98" si="12">SUM(C5:C97)</f>
+        <v>181</v>
+      </c>
+      <c r="D98" s="34">
         <f t="shared" si="12"/>
-        <v>149</v>
-      </c>
-      <c r="E95" s="34">
+        <v>156</v>
+      </c>
+      <c r="E98" s="34">
         <f t="shared" si="12"/>
-        <v>159</v>
-      </c>
-      <c r="F95" s="34">
+        <v>180</v>
+      </c>
+      <c r="F98" s="34">
         <f t="shared" si="12"/>
-        <v>146.5</v>
-      </c>
-      <c r="G95" s="34">
+        <v>153.5</v>
+      </c>
+      <c r="G98" s="34">
         <f t="shared" si="12"/>
         <v>63.5</v>
       </c>
-      <c r="H95" s="34">
+      <c r="H98" s="34">
         <f t="shared" si="12"/>
         <v>51</v>
       </c>
-      <c r="I95" s="34">
+      <c r="I98" s="34">
         <f t="shared" si="12"/>
-        <v>158.5</v>
-      </c>
-      <c r="J95" s="34">
+        <v>179.5</v>
+      </c>
+      <c r="J98" s="34">
         <f t="shared" si="12"/>
-        <v>144.5</v>
-      </c>
-      <c r="K95" s="34"/>
-      <c r="L95" s="34"/>
-      <c r="M95" s="32">
-        <f>C95+E95+G95+I95+K95</f>
-        <v>541</v>
-      </c>
-      <c r="N95" s="34">
-        <f>D95+F95+H95+J95+L95</f>
-        <v>491</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B96" s="33" t="s">
+        <v>152.5</v>
+      </c>
+      <c r="K98" s="34"/>
+      <c r="L98" s="34"/>
+      <c r="M98" s="32">
+        <f>C98+E98+G98+I98+K98</f>
+        <v>604</v>
+      </c>
+      <c r="N98" s="34">
+        <f>D98+F98+H98+J98+L98</f>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B99" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="K96" s="43"/>
+      <c r="K99" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4585,6 +4691,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
+    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
+    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D777D35650D3B43A23D41664AA30BC5" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="7f80e5700d93aba1c148b391c267eb5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ab5e87a-ed8e-45a5-9793-059f67398425" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e36a552b910c1cdf142adc90bba5ebe9" ns2:_="">
     <xsd:import namespace="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
@@ -4745,30 +4870,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
-    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
-    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6B4BC2B-47EC-4A4E-997D-A663CFE6E409}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4786,30 +4916,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
urenverandwoording en websocket update
</commit_message>
<xml_diff>
--- a/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
+++ b/docs/Uren_Verantwoording/Urenverantwoording Team 4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="94">
   <si>
     <t>Omschrijving activiteit</t>
   </si>
@@ -1109,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N99"/>
+  <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J95" sqref="J95"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H103" sqref="H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3747,7 +3747,7 @@
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
       <c r="M72" s="30">
-        <f t="shared" ref="M72:M97" si="11">C72+E72+G72+I72+K72</f>
+        <f t="shared" ref="M72:M100" si="11">C72+E72+G72+I72+K72</f>
         <v>12</v>
       </c>
       <c r="N72" s="2">
@@ -4534,11 +4534,15 @@
       <c r="C95" s="57">
         <v>7</v>
       </c>
-      <c r="D95" s="57"/>
+      <c r="D95" s="57">
+        <v>6</v>
+      </c>
       <c r="E95" s="38">
         <v>7</v>
       </c>
-      <c r="F95" s="38"/>
+      <c r="F95" s="38">
+        <v>6</v>
+      </c>
       <c r="G95" s="58">
         <v>0</v>
       </c>
@@ -4548,7 +4552,9 @@
       <c r="I95" s="38">
         <v>7</v>
       </c>
-      <c r="J95" s="38"/>
+      <c r="J95" s="38">
+        <v>6</v>
+      </c>
       <c r="K95" s="8"/>
       <c r="L95" s="8"/>
       <c r="M95" s="30"/>
@@ -4564,11 +4570,15 @@
       <c r="C96" s="57">
         <v>7</v>
       </c>
-      <c r="D96" s="57"/>
+      <c r="D96" s="57">
+        <v>6</v>
+      </c>
       <c r="E96" s="38">
         <v>7</v>
       </c>
-      <c r="F96" s="38"/>
+      <c r="F96" s="38">
+        <v>6</v>
+      </c>
       <c r="G96" s="58">
         <v>0</v>
       </c>
@@ -4578,86 +4588,172 @@
       <c r="I96" s="38">
         <v>7</v>
       </c>
-      <c r="J96" s="38"/>
+      <c r="J96" s="38">
+        <v>6</v>
+      </c>
       <c r="K96" s="8"/>
       <c r="L96" s="8"/>
       <c r="M96" s="30"/>
       <c r="N96" s="2"/>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A97" s="10"/>
-      <c r="B97" s="12"/>
-      <c r="C97" s="23"/>
-      <c r="D97" s="23"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="10"/>
-      <c r="G97" s="18">
-        <v>0</v>
-      </c>
-      <c r="H97" s="18">
-        <v>0</v>
-      </c>
-      <c r="I97" s="10"/>
-      <c r="J97" s="10"/>
+      <c r="A97" s="78"/>
+      <c r="B97" s="53"/>
+      <c r="C97" s="57"/>
+      <c r="D97" s="57"/>
+      <c r="E97" s="38"/>
+      <c r="F97" s="38"/>
+      <c r="G97" s="58"/>
+      <c r="H97" s="58"/>
+      <c r="I97" s="38"/>
+      <c r="J97" s="38"/>
       <c r="K97" s="8"/>
       <c r="L97" s="8"/>
-      <c r="M97" s="31">
+      <c r="M97" s="30"/>
+      <c r="N97" s="2"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="78">
+        <v>42431</v>
+      </c>
+      <c r="B98" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C98" s="57">
+        <v>7</v>
+      </c>
+      <c r="D98" s="57">
+        <v>6</v>
+      </c>
+      <c r="E98" s="38">
+        <v>7</v>
+      </c>
+      <c r="F98" s="38">
+        <v>6</v>
+      </c>
+      <c r="G98" s="58">
+        <v>0</v>
+      </c>
+      <c r="H98" s="58">
+        <v>0</v>
+      </c>
+      <c r="I98" s="38">
+        <v>7</v>
+      </c>
+      <c r="J98" s="38">
+        <v>8.5</v>
+      </c>
+      <c r="K98" s="8"/>
+      <c r="L98" s="8"/>
+      <c r="M98" s="30"/>
+      <c r="N98" s="2"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" s="78">
+        <v>42438</v>
+      </c>
+      <c r="B99" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C99" s="57">
+        <v>7</v>
+      </c>
+      <c r="D99" s="57">
+        <v>6</v>
+      </c>
+      <c r="E99" s="38">
+        <v>7</v>
+      </c>
+      <c r="F99" s="38">
+        <v>6</v>
+      </c>
+      <c r="G99" s="58">
+        <v>0</v>
+      </c>
+      <c r="H99" s="58">
+        <v>0</v>
+      </c>
+      <c r="I99" s="38">
+        <v>7</v>
+      </c>
+      <c r="J99" s="38">
+        <v>6</v>
+      </c>
+      <c r="K99" s="8"/>
+      <c r="L99" s="8"/>
+      <c r="M99" s="30"/>
+      <c r="N99" s="2"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" s="10"/>
+      <c r="B100" s="12"/>
+      <c r="C100" s="23"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="18"/>
+      <c r="H100" s="18"/>
+      <c r="I100" s="10"/>
+      <c r="J100" s="10"/>
+      <c r="K100" s="8"/>
+      <c r="L100" s="8"/>
+      <c r="M100" s="31">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N97" s="11"/>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A98" s="32"/>
-      <c r="B98" s="10"/>
-      <c r="C98" s="34">
-        <f t="shared" ref="C98:J98" si="12">SUM(C5:C97)</f>
-        <v>181</v>
-      </c>
-      <c r="D98" s="34">
-        <f t="shared" si="12"/>
-        <v>156</v>
-      </c>
-      <c r="E98" s="34">
+      <c r="N100" s="11"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A101" s="32"/>
+      <c r="B101" s="10"/>
+      <c r="C101" s="34">
+        <f t="shared" ref="C101:J101" si="12">SUM(C5:C100)</f>
+        <v>195</v>
+      </c>
+      <c r="D101" s="34">
         <f t="shared" si="12"/>
         <v>180</v>
       </c>
-      <c r="F98" s="34">
+      <c r="E101" s="34">
         <f t="shared" si="12"/>
-        <v>153.5</v>
-      </c>
-      <c r="G98" s="34">
+        <v>194</v>
+      </c>
+      <c r="F101" s="34">
+        <f t="shared" si="12"/>
+        <v>177.5</v>
+      </c>
+      <c r="G101" s="34">
         <f t="shared" si="12"/>
         <v>63.5</v>
       </c>
-      <c r="H98" s="34">
+      <c r="H101" s="34">
         <f t="shared" si="12"/>
         <v>51</v>
       </c>
-      <c r="I98" s="34">
+      <c r="I101" s="34">
         <f t="shared" si="12"/>
-        <v>179.5</v>
-      </c>
-      <c r="J98" s="34">
+        <v>193.5</v>
+      </c>
+      <c r="J101" s="34">
         <f t="shared" si="12"/>
-        <v>152.5</v>
-      </c>
-      <c r="K98" s="34"/>
-      <c r="L98" s="34"/>
-      <c r="M98" s="32">
-        <f>C98+E98+G98+I98+K98</f>
-        <v>604</v>
-      </c>
-      <c r="N98" s="34">
-        <f>D98+F98+H98+J98+L98</f>
-        <v>513</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B99" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="K101" s="34"/>
+      <c r="L101" s="34"/>
+      <c r="M101" s="32">
+        <f>C101+E101+G101+I101+K101</f>
+        <v>646</v>
+      </c>
+      <c r="N101" s="34">
+        <f>D101+F101+H101+J101+L101</f>
+        <v>587.5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B102" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="K99" s="43"/>
+      <c r="K102" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4691,25 +4787,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
-    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
-    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D777D35650D3B43A23D41664AA30BC5" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="7f80e5700d93aba1c148b391c267eb5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ab5e87a-ed8e-45a5-9793-059f67398425" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e36a552b910c1cdf142adc90bba5ebe9" ns2:_="">
     <xsd:import namespace="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
@@ -4870,35 +4947,30 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
+    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
+    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6B4BC2B-47EC-4A4E-997D-A663CFE6E409}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4916,6 +4988,30 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
   <ds:schemaRefs>

</xml_diff>